<commit_message>
Update du.xlsx (FOR 19 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sherminliam/Documents/School Work/IS212/G5T7/SECRET-BIOS/metrics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF79695-D9F2-084C-9FE1-D5F60CEA7227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606F39DE-AF1E-9540-B402-88D450661B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="5180" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="96">
   <si>
     <t>Question</t>
   </si>
@@ -10865,10 +10865,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10940,7 +10940,9 @@
       <c r="G3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -10963,7 +10965,9 @@
       <c r="G4" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -10986,7 +10990,9 @@
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11011,7 +11017,9 @@
       <c r="G6" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11034,7 +11042,9 @@
       <c r="G7" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11057,7 +11067,9 @@
       <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11082,7 +11094,9 @@
       <c r="G9" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11105,7 +11119,9 @@
       <c r="G10" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11128,7 +11144,9 @@
       <c r="G11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11153,7 +11171,9 @@
       <c r="G12" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11176,7 +11196,9 @@
       <c r="G13" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11199,7 +11221,9 @@
       <c r="G14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11224,7 +11248,9 @@
       <c r="G15" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11247,7 +11273,9 @@
       <c r="G16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11270,7 +11298,9 @@
       <c r="G17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I17" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update du.xlsx (FOR 20 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606F39DE-AF1E-9540-B402-88D450661B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012E6382-2D63-A04C-B275-6019BEAE552E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="5180" windowWidth="28800" windowHeight="16520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="98">
   <si>
     <t>Question</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>Plan for Iteration 3 tasks and its allocation</t>
+  </si>
+  <si>
+    <t>Clear round function (round 2)</t>
+  </si>
+  <si>
+    <t>Plan json checker functions' logic flow</t>
   </si>
 </sst>
 </file>
@@ -10868,7 +10874,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10943,7 +10949,9 @@
       <c r="H3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -10968,7 +10976,9 @@
       <c r="H4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -10993,7 +11003,9 @@
       <c r="H5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -11020,7 +11032,9 @@
       <c r="H6" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
@@ -11045,7 +11059,9 @@
       <c r="H7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -11070,7 +11086,9 @@
       <c r="H8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -11097,7 +11115,9 @@
       <c r="H9" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
@@ -11122,7 +11142,9 @@
       <c r="H10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
@@ -11147,7 +11169,9 @@
       <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
@@ -11174,7 +11198,9 @@
       <c r="H12" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
@@ -11199,7 +11225,9 @@
       <c r="H13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -11224,7 +11252,9 @@
       <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -11251,7 +11281,9 @@
       <c r="H15" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
@@ -11276,7 +11308,9 @@
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -11301,7 +11335,9 @@
       <c r="H17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Update du.xlsx (FOR 21 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012E6382-2D63-A04C-B275-6019BEAE552E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF2D4D-B0CF-7B49-AA34-B9043E16C752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="100">
   <si>
     <t>Question</t>
   </si>
@@ -341,6 +341,12 @@
   </si>
   <si>
     <t>Plan json checker functions' logic flow</t>
+  </si>
+  <si>
+    <t>Determine critical path for Iteration 3</t>
+  </si>
+  <si>
+    <t>Combine clear round function</t>
   </si>
 </sst>
 </file>
@@ -10870,11 +10876,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A70D3C-0BC5-2A46-9E56-0CDA371EBA40}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11358,11 +11364,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F80F15-7EDB-A24D-9E12-CEF767B2E501}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11419,7 +11425,9 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -11432,7 +11440,9 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -11445,7 +11455,9 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -11460,7 +11472,9 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -11473,7 +11487,9 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -11486,7 +11502,9 @@
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -11501,7 +11519,9 @@
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -11514,7 +11534,9 @@
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -11527,7 +11549,9 @@
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -11542,7 +11566,9 @@
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -11555,7 +11581,9 @@
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -11568,7 +11596,9 @@
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -11583,7 +11613,9 @@
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -11596,7 +11628,9 @@
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -11609,7 +11643,9 @@
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (FOR 22 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF2D4D-B0CF-7B49-AA34-B9043E16C752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8193A0F0-B90C-9141-931F-BCFAE3214242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="101">
   <si>
     <t>Question</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>Combine clear round function</t>
+  </si>
+  <si>
+    <t>View bidding function</t>
   </si>
 </sst>
 </file>
@@ -10880,7 +10883,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3:I17"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11365,10 +11368,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11428,7 +11431,9 @@
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>98</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -11443,7 +11448,9 @@
       <c r="C4" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -11458,7 +11465,9 @@
       <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -11475,7 +11484,9 @@
       <c r="C6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -11490,7 +11501,9 @@
       <c r="C7" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -11505,7 +11518,9 @@
       <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -11522,7 +11537,9 @@
       <c r="C9" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>99</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -11537,7 +11554,9 @@
       <c r="C10" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -11552,7 +11571,9 @@
       <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -11569,7 +11590,9 @@
       <c r="C12" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -11584,7 +11607,9 @@
       <c r="C13" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -11599,7 +11624,9 @@
       <c r="C14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -11616,7 +11643,9 @@
       <c r="C15" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -11631,7 +11660,9 @@
       <c r="C16" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -11646,7 +11677,9 @@
       <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (FOR 23 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8193A0F0-B90C-9141-931F-BCFAE3214242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60D91FB-695E-8349-AED2-6B011997AB22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="101">
   <si>
     <t>Question</t>
   </si>
@@ -11371,7 +11371,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11434,7 +11434,9 @@
       <c r="D3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -11451,7 +11453,9 @@
       <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -11468,7 +11472,9 @@
       <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -11487,7 +11493,9 @@
       <c r="D6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -11504,7 +11512,9 @@
       <c r="D7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -11521,7 +11531,9 @@
       <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -11540,7 +11552,9 @@
       <c r="D9" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -11557,7 +11571,9 @@
       <c r="D10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -11574,7 +11590,9 @@
       <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -11593,7 +11611,9 @@
       <c r="D12" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -11610,7 +11630,9 @@
       <c r="D13" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -11627,7 +11649,9 @@
       <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -11646,7 +11670,9 @@
       <c r="D15" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -11663,7 +11689,9 @@
       <c r="D16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -11680,7 +11708,9 @@
       <c r="D17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (FOR 24 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60D91FB-695E-8349-AED2-6B011997AB22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8029398A-648B-DD4B-97B5-84602E46A35C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="104">
   <si>
     <t>Question</t>
   </si>
@@ -350,6 +350,15 @@
   </si>
   <si>
     <t>View bidding function</t>
+  </si>
+  <si>
+    <t>Start round, stop round json checker</t>
+  </si>
+  <si>
+    <t>Dump table, user, bid, section, bid status json checker</t>
+  </si>
+  <si>
+    <t>Plan and allocate functions to the team to test</t>
   </si>
 </sst>
 </file>
@@ -11368,10 +11377,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11437,7 +11446,9 @@
       <c r="E3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -11456,7 +11467,9 @@
       <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -11475,7 +11488,9 @@
       <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -11496,7 +11511,9 @@
       <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -11515,7 +11532,9 @@
       <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -11534,7 +11553,9 @@
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -11555,7 +11576,9 @@
       <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -11574,7 +11597,9 @@
       <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -11593,7 +11618,9 @@
       <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -11614,7 +11641,9 @@
       <c r="E12" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -11633,7 +11662,9 @@
       <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -11652,7 +11683,9 @@
       <c r="E14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -11673,7 +11706,9 @@
       <c r="E15" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -11692,7 +11727,9 @@
       <c r="E16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -11711,7 +11748,9 @@
       <c r="E17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (FOR 25 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8029398A-648B-DD4B-97B5-84602E46A35C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6840954-063F-154A-9175-C596A888FD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="104">
   <si>
     <t>Question</t>
   </si>
@@ -11377,10 +11377,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11449,7 +11449,9 @@
       <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
@@ -11470,7 +11472,9 @@
       <c r="F4" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
@@ -11491,7 +11495,9 @@
       <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
@@ -11514,7 +11520,9 @@
       <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
@@ -11535,7 +11543,9 @@
       <c r="F7" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
@@ -11556,7 +11566,9 @@
       <c r="F8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
@@ -11579,7 +11591,9 @@
       <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
@@ -11600,7 +11614,9 @@
       <c r="F10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
@@ -11621,7 +11637,9 @@
       <c r="F11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
@@ -11644,7 +11662,9 @@
       <c r="F12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
@@ -11665,7 +11685,9 @@
       <c r="F13" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
@@ -11686,7 +11708,9 @@
       <c r="F14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
@@ -11709,7 +11733,9 @@
       <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
@@ -11730,7 +11756,9 @@
       <c r="F16" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
@@ -11751,7 +11779,9 @@
       <c r="F17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update du.xlsx (FOR 26 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5E5751-8CD2-C64A-B92F-30C0C36E6A35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE4C6EB-9ED2-A940-86EB-307A44521BA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="110">
   <si>
     <t>Question</t>
   </si>
@@ -359,6 +359,24 @@
   </si>
   <si>
     <t>Plan and allocate functions to the team to test</t>
+  </si>
+  <si>
+    <t>Commits done the day before were accidentally reverted</t>
+  </si>
+  <si>
+    <t>Dump, start/clear round, drop bid testcases</t>
+  </si>
+  <si>
+    <t>Dump, bootstrap, place bid testcases</t>
+  </si>
+  <si>
+    <t>Start/clear round, drop section, bootstrap testcases</t>
+  </si>
+  <si>
+    <t>Drop bid, drop section, login testcases</t>
+  </si>
+  <si>
+    <t>Dump, drop bid, place bid testcases</t>
   </si>
 </sst>
 </file>
@@ -11377,10 +11395,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11452,7 +11470,9 @@
       <c r="G3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11475,7 +11495,9 @@
       <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11498,7 +11520,9 @@
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11523,7 +11547,9 @@
       <c r="G6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11546,7 +11572,9 @@
       <c r="G7" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11569,7 +11597,9 @@
       <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11594,7 +11624,9 @@
       <c r="G9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11617,7 +11649,9 @@
       <c r="G10" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11640,7 +11674,9 @@
       <c r="G11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11665,7 +11701,9 @@
       <c r="G12" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11688,7 +11726,9 @@
       <c r="G13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11711,7 +11751,9 @@
       <c r="G14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11736,7 +11778,9 @@
       <c r="G15" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11759,7 +11803,9 @@
       <c r="G16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -11782,7 +11828,9 @@
       <c r="G17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I17" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update du.xlsx (FOR 27 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE4C6EB-9ED2-A940-86EB-307A44521BA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAC520E-67E1-EC4E-A06E-20E1E220BA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="112">
   <si>
     <t>Question</t>
   </si>
@@ -377,6 +377,12 @@
   </si>
   <si>
     <t>Dump, drop bid, place bid testcases</t>
+  </si>
+  <si>
+    <t>Debugging Session</t>
+  </si>
+  <si>
+    <t>Run testcases + regression testing</t>
   </si>
 </sst>
 </file>
@@ -11395,10 +11401,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11473,7 +11479,9 @@
       <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -11498,7 +11506,9 @@
       <c r="H4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -11523,7 +11533,9 @@
       <c r="H5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -11550,7 +11562,9 @@
       <c r="H6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
@@ -11575,7 +11589,9 @@
       <c r="H7" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -11600,7 +11616,9 @@
       <c r="H8" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -11627,7 +11645,9 @@
       <c r="H9" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
@@ -11652,7 +11672,9 @@
       <c r="H10" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
@@ -11677,7 +11699,9 @@
       <c r="H11" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
@@ -11704,7 +11728,9 @@
       <c r="H12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
@@ -11729,7 +11755,9 @@
       <c r="H13" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -11754,7 +11782,9 @@
       <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -11781,7 +11811,9 @@
       <c r="H15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
@@ -11806,7 +11838,9 @@
       <c r="H16" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -11831,7 +11865,9 @@
       <c r="H17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Update du.xlsx (FOR 28 OCT)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weichen/Documents/GitHub/SECRET-BIOS/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAC520E-67E1-EC4E-A06E-20E1E220BA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A8B980-F9EA-0341-BF66-DC50FC939C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="112">
   <si>
     <t>Question</t>
   </si>
@@ -11400,11 +11400,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F80F15-7EDB-A24D-9E12-CEF767B2E501}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11888,11 +11888,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A34FEB-DAD5-9143-886E-3EB69BEEF73E}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11949,7 +11949,9 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -11962,7 +11964,9 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -11975,7 +11979,9 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -11990,7 +11996,9 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -12003,7 +12011,9 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -12016,7 +12026,9 @@
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -12031,7 +12043,9 @@
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -12044,7 +12058,9 @@
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -12057,7 +12073,9 @@
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -12072,7 +12090,9 @@
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -12085,7 +12105,9 @@
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -12098,7 +12120,9 @@
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -12113,7 +12137,9 @@
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -12126,7 +12152,9 @@
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -12139,7 +12167,9 @@
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (2 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397F089F-638D-4470-B6FD-E51FE2DEC98B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CB2F72-DE6D-4199-889D-8F6525B5F73C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="116">
   <si>
     <t>Question</t>
   </si>
@@ -11928,10 +11928,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:G17"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12003,7 +12003,9 @@
       <c r="G3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12026,7 +12028,9 @@
       <c r="G4" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12074,7 +12078,9 @@
       <c r="G6" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12097,7 +12103,9 @@
       <c r="G7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12120,7 +12128,9 @@
       <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12145,7 +12155,9 @@
       <c r="G9" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12168,7 +12180,9 @@
       <c r="G10" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12191,7 +12205,9 @@
       <c r="G11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12216,7 +12232,9 @@
       <c r="G12" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12239,7 +12257,9 @@
       <c r="G13" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12262,7 +12282,9 @@
       <c r="G14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12287,7 +12309,9 @@
       <c r="G15" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>115</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12310,7 +12334,9 @@
       <c r="G16" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12333,7 +12359,9 @@
       <c r="G17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I17" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Update du.xlsx (2 Nov)"
This reverts commit 6a9d431c2bc08090a43bb249cc69f62f48545054.
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F8725-B777-460E-8740-1D409055DEE5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CB2F72-DE6D-4199-889D-8F6525B5F73C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="116">
   <si>
     <t>Question</t>
   </si>
@@ -11928,10 +11928,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12006,9 +12006,7 @@
       <c r="H3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -12033,9 +12031,7 @@
       <c r="H4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -12058,9 +12054,7 @@
         <v>21</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -12087,9 +12081,7 @@
       <c r="H6" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
@@ -12114,9 +12106,7 @@
       <c r="H7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -12141,9 +12131,7 @@
       <c r="H8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -12170,9 +12158,7 @@
       <c r="H9" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
@@ -12197,9 +12183,7 @@
       <c r="H10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
@@ -12224,9 +12208,7 @@
       <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
@@ -12253,9 +12235,7 @@
       <c r="H12" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
@@ -12280,9 +12260,7 @@
       <c r="H13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -12307,9 +12285,7 @@
       <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -12336,9 +12312,7 @@
       <c r="H15" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
@@ -12363,9 +12337,7 @@
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -12390,9 +12362,7 @@
       <c r="H17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="I17" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Update du.xlsx (3 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CB2F72-DE6D-4199-889D-8F6525B5F73C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87546359-DA2A-407A-9745-05B4D2915633}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="116">
   <si>
     <t>Question</t>
   </si>
@@ -11931,7 +11931,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12006,7 +12006,9 @@
       <c r="H3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -12031,7 +12033,9 @@
       <c r="H4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -12054,7 +12058,9 @@
         <v>21</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -12081,7 +12087,9 @@
       <c r="H6" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
@@ -12106,7 +12114,9 @@
       <c r="H7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -12131,7 +12141,9 @@
       <c r="H8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -12158,7 +12170,9 @@
       <c r="H9" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
@@ -12183,7 +12197,9 @@
       <c r="H10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
@@ -12208,7 +12224,9 @@
       <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
@@ -12235,7 +12253,9 @@
       <c r="H12" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
@@ -12260,7 +12280,9 @@
       <c r="H13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -12285,7 +12307,9 @@
       <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -12312,7 +12336,9 @@
       <c r="H15" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
@@ -12337,7 +12363,9 @@
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -12362,7 +12390,9 @@
       <c r="H17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Update du.xlsx (4 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87546359-DA2A-407A-9745-05B4D2915633}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E28ABE-00C5-4189-BAF1-896F460610CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="116">
   <si>
     <t>Question</t>
   </si>
@@ -11927,7 +11927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75A34FEB-DAD5-9143-886E-3EB69BEEF73E}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -12417,11 +12417,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F311D3-DB5D-434C-A138-D6E762210AAD}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:I1"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12478,7 +12478,9 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -12491,7 +12493,9 @@
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -12504,7 +12508,9 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -12519,7 +12525,9 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -12532,7 +12540,9 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -12545,7 +12555,9 @@
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -12560,7 +12572,9 @@
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -12573,7 +12587,9 @@
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -12586,7 +12602,9 @@
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -12601,7 +12619,9 @@
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -12614,7 +12634,9 @@
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -12627,7 +12649,9 @@
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -12642,7 +12666,9 @@
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -12655,7 +12681,9 @@
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -12668,7 +12696,9 @@
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (5 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E28ABE-00C5-4189-BAF1-896F460610CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36AF385-ED14-4372-9E98-F60761520476}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="116">
   <si>
     <t>Question</t>
   </si>
@@ -12421,7 +12421,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12481,7 +12481,9 @@
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -12496,7 +12498,9 @@
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -12511,7 +12515,9 @@
       <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -12528,7 +12534,9 @@
       <c r="C6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -12543,7 +12551,9 @@
       <c r="C7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -12558,7 +12568,9 @@
       <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -12575,7 +12587,9 @@
       <c r="C9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -12590,7 +12604,9 @@
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -12605,7 +12621,9 @@
       <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -12622,7 +12640,9 @@
       <c r="C12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -12637,7 +12657,9 @@
       <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -12652,7 +12674,9 @@
       <c r="C14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -12669,7 +12693,9 @@
       <c r="C15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -12684,7 +12710,9 @@
       <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -12699,7 +12727,9 @@
       <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (6 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36AF385-ED14-4372-9E98-F60761520476}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B072EA5-7D5A-4B4A-85B2-5B51F5CDE6C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="116">
   <si>
     <t>Question</t>
   </si>
@@ -12417,11 +12417,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F311D3-DB5D-434C-A138-D6E762210AAD}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3:D17"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12484,7 +12484,9 @@
       <c r="D3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -12501,7 +12503,9 @@
       <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -12518,7 +12522,9 @@
       <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -12537,7 +12543,9 @@
       <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -12554,7 +12562,9 @@
       <c r="D7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -12571,7 +12581,9 @@
       <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -12590,7 +12602,9 @@
       <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -12607,7 +12621,9 @@
       <c r="D10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -12624,7 +12640,9 @@
       <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -12643,7 +12661,9 @@
       <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -12660,7 +12680,9 @@
       <c r="D13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -12677,7 +12699,9 @@
       <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -12696,7 +12720,9 @@
       <c r="D15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -12713,7 +12739,9 @@
       <c r="D16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -12730,7 +12758,9 @@
       <c r="D17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (7 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B072EA5-7D5A-4B4A-85B2-5B51F5CDE6C8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0513EF96-43BE-4095-B517-0B87CB5A094A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="116">
   <si>
     <t>Question</t>
   </si>
@@ -12421,7 +12421,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12487,7 +12487,9 @@
       <c r="E3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -12506,7 +12508,9 @@
       <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -12525,7 +12529,9 @@
       <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -12546,7 +12552,9 @@
       <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -12565,7 +12573,9 @@
       <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -12584,7 +12594,9 @@
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -12605,7 +12617,9 @@
       <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -12624,7 +12638,9 @@
       <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -12643,7 +12659,9 @@
       <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -12664,7 +12682,9 @@
       <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -12683,7 +12703,9 @@
       <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -12702,7 +12724,9 @@
       <c r="E14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -12723,7 +12747,9 @@
       <c r="E15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -12742,7 +12768,9 @@
       <c r="E16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -12761,7 +12789,9 @@
       <c r="E17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (8 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0513EF96-43BE-4095-B517-0B87CB5A094A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D7B564-A190-4745-9D31-45A95D4EE7FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="117">
   <si>
     <t>Question</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>Plan for Iteration 4 tasks and its allocation</t>
+  </si>
+  <si>
+    <t>Prepare additional testcases, run testcases + regression testing</t>
   </si>
 </sst>
 </file>
@@ -12418,10 +12421,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3:F17"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12490,7 +12493,9 @@
       <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
@@ -12511,7 +12516,9 @@
       <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
@@ -12532,7 +12539,9 @@
       <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
@@ -12555,7 +12564,9 @@
       <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
@@ -12576,7 +12587,9 @@
       <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
@@ -12597,7 +12610,9 @@
       <c r="F8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
@@ -12620,11 +12635,13 @@
       <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -12641,7 +12658,9 @@
       <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
@@ -12662,7 +12681,9 @@
       <c r="F11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
@@ -12685,7 +12706,9 @@
       <c r="F12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
@@ -12706,7 +12729,9 @@
       <c r="F13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
@@ -12727,7 +12752,9 @@
       <c r="F14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
@@ -12750,11 +12777,13 @@
       <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -12771,7 +12800,9 @@
       <c r="F16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
@@ -12792,7 +12823,9 @@
       <c r="F17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update du.xlsx (9 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D7B564-A190-4745-9D31-45A95D4EE7FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC50F791-B0A9-45DA-B05A-1A4AB35F5780}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="118">
   <si>
     <t>Question</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>Prepare additional testcases, run testcases + regression testing</t>
+  </si>
+  <si>
+    <t>Fix all bugs from UAT and testcases</t>
   </si>
 </sst>
 </file>
@@ -12424,7 +12427,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12496,7 +12499,9 @@
       <c r="G3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12519,7 +12524,9 @@
       <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12542,7 +12549,9 @@
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12567,7 +12576,9 @@
       <c r="G6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12590,7 +12601,9 @@
       <c r="G7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12613,10 +12626,12 @@
       <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -12638,7 +12653,9 @@
       <c r="G9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12661,7 +12678,9 @@
       <c r="G10" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12684,7 +12703,9 @@
       <c r="G11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12709,7 +12730,9 @@
       <c r="G12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12732,7 +12755,9 @@
       <c r="G13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12755,10 +12780,12 @@
       <c r="G14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>17</v>
       </c>
@@ -12780,7 +12807,9 @@
       <c r="G15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12803,7 +12832,9 @@
       <c r="G16" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12826,7 +12857,9 @@
       <c r="G17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I17" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update & edit du.xlsx (8. 9 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC50F791-B0A9-45DA-B05A-1A4AB35F5780}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEE6E62-672E-4CB3-9FF1-A698DA0072AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="120">
   <si>
     <t>Question</t>
   </si>
@@ -397,10 +397,18 @@
     <t>Plan for Iteration 4 tasks and its allocation</t>
   </si>
   <si>
-    <t>Prepare additional testcases, run testcases + regression testing</t>
+    <t>Fix all bugs from UAT and testcases</t>
   </si>
   <si>
-    <t>Fix all bugs from UAT and testcases</t>
+    <t>Run testcases + regression testing, Fix all bugs from UAT and testcases</t>
+  </si>
+  <si>
+    <t>Prepare additional testcases, 
+Fix all bugs from UAT and testcases</t>
+  </si>
+  <si>
+    <t>Prepare additional testcases, Run testcases + regression testing
+Fix all bugs from UAT and testcases</t>
   </si>
 </sst>
 </file>
@@ -12424,10 +12432,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12525,7 +12533,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I4" s="7"/>
     </row>
@@ -12602,7 +12610,7 @@
         <v>22</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I7" s="7"/>
     </row>
@@ -12654,7 +12662,7 @@
         <v>22</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="I9" s="7"/>
     </row>
@@ -12676,7 +12684,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>117</v>
@@ -12735,7 +12743,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
@@ -12756,7 +12764,7 @@
         <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I13" s="7"/>
     </row>
@@ -12808,11 +12816,11 @@
         <v>22</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -12830,10 +12838,10 @@
         <v>22</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I16" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update du.xlsx (10 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDEE6E62-672E-4CB3-9FF1-A698DA0072AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201308B4-A697-442B-A587-A8EFD10716EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="123">
   <si>
     <t>Question</t>
   </si>
@@ -409,6 +409,15 @@
   <si>
     <t>Prepare additional testcases, Run testcases + regression testing
 Fix all bugs from UAT and testcases</t>
+  </si>
+  <si>
+    <t>Deploy app</t>
+  </si>
+  <si>
+    <t>Test app on web server + debugging, prepare bug metrics</t>
+  </si>
+  <si>
+    <t>Prepare bug metrics, deploy app, Test app on web server + debugging, prepare bug metrics</t>
   </si>
 </sst>
 </file>
@@ -12435,7 +12444,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12510,7 +12519,9 @@
       <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -12535,7 +12546,9 @@
       <c r="H4" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -12560,7 +12573,9 @@
       <c r="H5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -12587,7 +12602,9 @@
       <c r="H6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
@@ -12612,7 +12629,9 @@
       <c r="H7" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -12637,9 +12656,11 @@
       <c r="H8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
@@ -12664,7 +12685,9 @@
       <c r="H9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
@@ -12689,7 +12712,9 @@
       <c r="H10" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
@@ -12714,9 +12739,11 @@
       <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
@@ -12741,7 +12768,9 @@
       <c r="H12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
@@ -12766,7 +12795,9 @@
       <c r="H13" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -12791,9 +12822,11 @@
       <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>17</v>
       </c>
@@ -12818,7 +12851,9 @@
       <c r="H15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
@@ -12843,7 +12878,9 @@
       <c r="H16" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -12868,7 +12905,9 @@
       <c r="H17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Update du.xlsx (11 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201308B4-A697-442B-A587-A8EFD10716EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9670B0-8E61-4852-B1AC-0666BCD27177}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="124">
   <si>
     <t>Question</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Prepare bug metrics, deploy app, Test app on web server + debugging, prepare bug metrics</t>
+  </si>
+  <si>
+    <t>Prepare for final submission and presentation slides</t>
   </si>
 </sst>
 </file>
@@ -12440,7 +12443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F311D3-DB5D-434C-A138-D6E762210AAD}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -12932,11 +12935,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B36927-73C5-5B47-AF35-F1F069D84D34}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12993,7 +12996,9 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -13001,12 +13006,14 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -13019,7 +13026,9 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -13034,7 +13043,9 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -13042,12 +13053,14 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -13060,7 +13073,9 @@
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -13068,14 +13083,16 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -13088,7 +13105,9 @@
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -13101,7 +13120,9 @@
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -13116,7 +13137,9 @@
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -13124,12 +13147,14 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -13142,7 +13167,9 @@
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -13150,14 +13177,16 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -13165,12 +13194,14 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -13183,7 +13214,9 @@
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (11 Nov edited)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9670B0-8E61-4852-B1AC-0666BCD27177}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC8FD75-EEF9-438A-8BC7-28C029F05778}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
     <t>Prepare bug metrics, deploy app, Test app on web server + debugging, prepare bug metrics</t>
   </si>
   <si>
-    <t>Prepare for final submission and presentation slides</t>
+    <t>Debug + update tescases</t>
   </si>
 </sst>
 </file>
@@ -12936,10 +12936,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13012,7 +13012,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -13106,7 +13106,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -13200,7 +13200,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (12 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC8FD75-EEF9-438A-8BC7-28C029F05778}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6E4430-C3C2-4F32-A79B-C77BC471C5F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="126">
   <si>
     <t>Question</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>Debug + update tescases</t>
+  </si>
+  <si>
+    <t>Update testcases, debug and prepare bug metrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploy app </t>
   </si>
 </sst>
 </file>
@@ -12936,10 +12942,10 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12999,7 +13005,9 @@
       <c r="C3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -13014,7 +13022,9 @@
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -13029,7 +13039,9 @@
       <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -13046,7 +13058,9 @@
       <c r="C6" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -13061,7 +13075,9 @@
       <c r="C7" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -13076,7 +13092,9 @@
       <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -13093,7 +13111,9 @@
       <c r="C9" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -13108,7 +13128,9 @@
       <c r="C10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -13123,7 +13145,9 @@
       <c r="C11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -13140,7 +13164,9 @@
       <c r="C12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>125</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -13155,7 +13181,9 @@
       <c r="C13" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -13170,7 +13198,9 @@
       <c r="C14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -13187,7 +13217,9 @@
       <c r="C15" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -13202,7 +13234,9 @@
       <c r="C16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -13217,7 +13251,9 @@
       <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (13 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6E4430-C3C2-4F32-A79B-C77BC471C5F0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA83701-F342-49A7-A526-07B552FA7FE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="125">
   <si>
     <t>Question</t>
   </si>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>Prepare bug metrics, deploy app, Test app on web server + debugging, prepare bug metrics</t>
-  </si>
-  <si>
-    <t>Debug + update tescases</t>
   </si>
   <si>
     <t>Update testcases, debug and prepare bug metrics</t>
@@ -12945,7 +12942,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12995,7 +12992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>14</v>
       </c>
@@ -13008,7 +13005,9 @@
       <c r="D3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -13025,7 +13024,9 @@
       <c r="D4" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -13042,13 +13043,15 @@
       <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>13</v>
       </c>
@@ -13061,7 +13064,9 @@
       <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -13073,12 +13078,14 @@
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -13095,7 +13102,9 @@
       <c r="D8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -13112,9 +13121,11 @@
         <v>121</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>123</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -13126,12 +13137,14 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -13148,7 +13161,9 @@
       <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -13165,9 +13180,11 @@
         <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -13179,12 +13196,14 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -13201,7 +13220,9 @@
       <c r="D14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -13218,9 +13239,11 @@
         <v>122</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="7"/>
+        <v>123</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -13232,12 +13255,14 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="7"/>
+        <v>121</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -13254,7 +13279,9 @@
       <c r="D17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>

</xml_diff>

<commit_message>
Update du.xlsx (14 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA83701-F342-49A7-A526-07B552FA7FE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6D3312-36E8-4FDA-8DA7-A2912AD5A54C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="125">
   <si>
     <t>Question</t>
   </si>
@@ -12942,7 +12942,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13008,7 +13008,9 @@
       <c r="E3" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -13027,7 +13029,9 @@
       <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -13046,7 +13050,9 @@
       <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -13067,7 +13073,9 @@
       <c r="E6" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -13086,7 +13094,9 @@
       <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -13105,7 +13115,9 @@
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
@@ -13126,7 +13138,9 @@
       <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -13145,7 +13159,9 @@
       <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -13164,7 +13180,9 @@
       <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -13185,7 +13203,9 @@
       <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -13204,7 +13224,9 @@
       <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -13223,7 +13245,9 @@
       <c r="E14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -13244,7 +13268,9 @@
       <c r="E15" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -13263,7 +13289,9 @@
       <c r="E16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -13282,7 +13310,9 @@
       <c r="E17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>

</xml_diff>

<commit_message>
Revert "Update du.xlsx (14 Nov)"
This reverts commit b5067381e8a69ca91aaf87fdc979e0b759f0053c.
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C28F87-EEE6-4740-84BF-CA0083418C18}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6D3312-36E8-4FDA-8DA7-A2912AD5A54C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Week 11" sheetId="7" r:id="rId7"/>
     <sheet name="Week 12" sheetId="8" r:id="rId8"/>
     <sheet name="Week 13" sheetId="9" r:id="rId9"/>
+    <sheet name="Week 14" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="125">
   <si>
     <t>Question</t>
   </si>
@@ -325,6 +326,9 @@
   </si>
   <si>
     <t>Week: 11 Nov to 17 Nov</t>
+  </si>
+  <si>
+    <t>Week: 18 Nov to 24 Nov</t>
   </si>
   <si>
     <t>App Demo &amp; Progress Update</t>
@@ -5268,6 +5272,288 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D329D56-B4E6-A741-8F1C-1B236FB18199}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="9" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;8 SMU Classification: Restricted&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810C4FA2-0B07-204A-901F-21D0E14895D7}">
   <dimension ref="A1:I1001"/>
@@ -10760,10 +11046,10 @@
         <v>87</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>22</v>
@@ -10784,10 +11070,10 @@
         <v>87</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>22</v>
@@ -10843,10 +11129,10 @@
         <v>87</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>22</v>
@@ -10867,16 +11153,16 @@
         <v>87</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -10926,10 +11212,10 @@
         <v>87</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>22</v>
@@ -10950,16 +11236,16 @@
         <v>87</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11009,10 +11295,10 @@
         <v>87</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>22</v>
@@ -11033,16 +11319,16 @@
         <v>87</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11092,10 +11378,10 @@
         <v>87</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>22</v>
@@ -11116,16 +11402,16 @@
         <v>87</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11243,7 +11529,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>22</v>
@@ -11252,13 +11538,13 @@
         <v>22</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11267,7 +11553,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>22</v>
@@ -11276,13 +11562,13 @@
         <v>22</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>84</v>
@@ -11323,10 +11609,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>22</v>
@@ -11338,10 +11624,10 @@
         <v>22</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11350,7 +11636,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>22</v>
@@ -11362,13 +11648,13 @@
         <v>22</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11392,7 +11678,7 @@
         <v>21</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>21</v>
@@ -11406,10 +11692,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
@@ -11421,10 +11707,10 @@
         <v>22</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11433,7 +11719,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>22</v>
@@ -11445,13 +11731,13 @@
         <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11475,7 +11761,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>21</v>
@@ -11489,25 +11775,25 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11516,25 +11802,25 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11572,25 +11858,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11599,25 +11885,25 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11738,16 +12024,16 @@
         <v>84</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>22</v>
@@ -11762,16 +12048,16 @@
         <v>84</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>22</v>
@@ -11813,22 +12099,22 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>22</v>
@@ -11840,19 +12126,19 @@
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>22</v>
@@ -11896,22 +12182,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>22</v>
@@ -11923,19 +12209,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>22</v>
@@ -11979,22 +12265,22 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>22</v>
@@ -12006,19 +12292,19 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>22</v>
@@ -12062,22 +12348,22 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>22</v>
@@ -12089,19 +12375,19 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>22</v>
@@ -12240,7 +12526,7 @@
         <v>22</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12264,7 +12550,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>22</v>
@@ -12323,7 +12609,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12347,10 +12633,10 @@
         <v>22</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12406,7 +12692,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12430,10 +12716,10 @@
         <v>22</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12489,7 +12775,7 @@
         <v>22</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12513,7 +12799,7 @@
         <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>22</v>
@@ -12572,7 +12858,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12596,10 +12882,10 @@
         <v>22</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12656,7 +12942,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12720,14 +13006,12 @@
         <v>22</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
@@ -12740,7 +13024,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>22</v>
@@ -12748,9 +13032,7 @@
       <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
@@ -12771,9 +13053,7 @@
       <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
@@ -12785,20 +13065,18 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
@@ -12811,7 +13089,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>22</v>
@@ -12819,9 +13097,7 @@
       <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
@@ -12842,9 +13118,7 @@
       <c r="F8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
@@ -12856,10 +13130,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
@@ -12867,9 +13141,7 @@
       <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
@@ -12879,7 +13151,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>22</v>
@@ -12890,9 +13162,7 @@
       <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
@@ -12913,9 +13183,7 @@
       <c r="F11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
@@ -12930,7 +13198,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>22</v>
@@ -12938,9 +13206,7 @@
       <c r="F12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
@@ -12950,7 +13216,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>22</v>
@@ -12961,9 +13227,7 @@
       <c r="F13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
@@ -12984,9 +13248,7 @@
       <c r="F14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
@@ -12998,20 +13260,18 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>120</v>
-      </c>
       <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
@@ -13021,10 +13281,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>22</v>
@@ -13032,9 +13292,7 @@
       <c r="F16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
@@ -13055,9 +13313,7 @@
       <c r="F17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update du.xlsx (15 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6D3312-36E8-4FDA-8DA7-A2912AD5A54C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E785EC-B3CE-4371-81F1-33C6D152F6DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="Week 11" sheetId="7" r:id="rId7"/>
     <sheet name="Week 12" sheetId="8" r:id="rId8"/>
     <sheet name="Week 13" sheetId="9" r:id="rId9"/>
-    <sheet name="Week 14" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="124">
   <si>
     <t>Question</t>
   </si>
@@ -326,9 +325,6 @@
   </si>
   <si>
     <t>Week: 11 Nov to 17 Nov</t>
-  </si>
-  <si>
-    <t>Week: 18 Nov to 24 Nov</t>
   </si>
   <si>
     <t>App Demo &amp; Progress Update</t>
@@ -5272,288 +5268,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D329D56-B4E6-A741-8F1C-1B236FB18199}">
-  <dimension ref="A1:I17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="9" width="28.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;8 SMU Classification: Restricted&amp;1#</oddHeader>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810C4FA2-0B07-204A-901F-21D0E14895D7}">
   <dimension ref="A1:I1001"/>
@@ -11046,10 +10760,10 @@
         <v>87</v>
       </c>
       <c r="G3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>22</v>
@@ -11070,10 +10784,10 @@
         <v>87</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>22</v>
@@ -11129,10 +10843,10 @@
         <v>87</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>22</v>
@@ -11153,16 +10867,16 @@
         <v>87</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11212,10 +10926,10 @@
         <v>87</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>22</v>
@@ -11236,16 +10950,16 @@
         <v>87</v>
       </c>
       <c r="F10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11295,10 +11009,10 @@
         <v>87</v>
       </c>
       <c r="G12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>22</v>
@@ -11319,16 +11033,16 @@
         <v>87</v>
       </c>
       <c r="F13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="H13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11378,10 +11092,10 @@
         <v>87</v>
       </c>
       <c r="G15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>22</v>
@@ -11402,16 +11116,16 @@
         <v>87</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="H16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11529,7 +11243,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>22</v>
@@ -11538,13 +11252,13 @@
         <v>22</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11553,7 +11267,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>22</v>
@@ -11562,13 +11276,13 @@
         <v>22</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>84</v>
@@ -11609,10 +11323,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>22</v>
@@ -11624,10 +11338,10 @@
         <v>22</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11636,7 +11350,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>22</v>
@@ -11648,13 +11362,13 @@
         <v>22</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11678,7 +11392,7 @@
         <v>21</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>21</v>
@@ -11692,10 +11406,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
@@ -11707,10 +11421,10 @@
         <v>22</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11719,7 +11433,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>22</v>
@@ -11731,13 +11445,13 @@
         <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11761,7 +11475,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>21</v>
@@ -11775,25 +11489,25 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="H12" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11802,25 +11516,25 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="G13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11858,25 +11572,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="H15" s="7" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -11885,25 +11599,25 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="G16" s="7" t="s">
         <v>22</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12024,16 +11738,16 @@
         <v>84</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>22</v>
@@ -12048,16 +11762,16 @@
         <v>84</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>22</v>
@@ -12099,22 +11813,22 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>22</v>
@@ -12126,19 +11840,19 @@
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>22</v>
@@ -12182,22 +11896,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="G9" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>22</v>
@@ -12209,19 +11923,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>22</v>
@@ -12265,22 +11979,22 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>22</v>
@@ -12292,19 +12006,19 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>22</v>
@@ -12348,22 +12062,22 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>22</v>
@@ -12375,19 +12089,19 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>22</v>
@@ -12526,7 +12240,7 @@
         <v>22</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12550,7 +12264,7 @@
         <v>22</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>22</v>
@@ -12609,7 +12323,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12633,10 +12347,10 @@
         <v>22</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12692,7 +12406,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12716,10 +12430,10 @@
         <v>22</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12775,7 +12489,7 @@
         <v>22</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12799,7 +12513,7 @@
         <v>22</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>22</v>
@@ -12858,7 +12572,7 @@
         <v>22</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12882,10 +12596,10 @@
         <v>22</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12942,7 +12656,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3:F17"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13006,12 +12720,14 @@
         <v>22</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
@@ -13024,7 +12740,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>22</v>
@@ -13032,7 +12748,9 @@
       <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
@@ -13053,7 +12771,9 @@
       <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
@@ -13065,18 +12785,20 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="F6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
@@ -13089,7 +12811,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>22</v>
@@ -13097,7 +12819,9 @@
       <c r="F7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
@@ -13118,7 +12842,9 @@
       <c r="F8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
@@ -13130,10 +12856,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>22</v>
@@ -13141,7 +12867,9 @@
       <c r="F9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
@@ -13151,7 +12879,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>22</v>
@@ -13162,7 +12890,9 @@
       <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
@@ -13183,7 +12913,9 @@
       <c r="F11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
@@ -13198,7 +12930,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>22</v>
@@ -13206,7 +12938,9 @@
       <c r="F12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="7"/>
+      <c r="G12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
@@ -13216,7 +12950,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>22</v>
@@ -13227,7 +12961,9 @@
       <c r="F13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
@@ -13248,7 +12984,9 @@
       <c r="F14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
@@ -13260,18 +12998,20 @@
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>123</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
@@ -13281,10 +13021,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>22</v>
@@ -13292,7 +13032,9 @@
       <c r="F16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
@@ -13313,7 +13055,9 @@
       <c r="F17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update du.xlsx (16 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E785EC-B3CE-4371-81F1-33C6D152F6DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DAB711-2FD4-4DB2-861C-73F2DABC2F66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="125">
   <si>
     <t>Question</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t xml:space="preserve">Deploy app </t>
+  </si>
+  <si>
+    <t>Prepare for final submission and presentation slides</t>
   </si>
 </sst>
 </file>
@@ -12656,7 +12659,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12728,7 +12731,9 @@
       <c r="G3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12751,7 +12756,9 @@
       <c r="G4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12774,7 +12781,9 @@
       <c r="G5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -12799,7 +12808,9 @@
       <c r="G6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12822,7 +12833,9 @@
       <c r="G7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12845,7 +12858,9 @@
       <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12870,10 +12885,12 @@
       <c r="G9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="4" t="s">
         <v>8</v>
@@ -12893,7 +12910,9 @@
       <c r="G10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12916,7 +12935,9 @@
       <c r="G11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12941,7 +12962,9 @@
       <c r="G12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.2">
@@ -12964,7 +12987,9 @@
       <c r="G13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -12987,7 +13012,9 @@
       <c r="G14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13012,7 +13039,9 @@
       <c r="G15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13035,7 +13064,9 @@
       <c r="G16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
@@ -13058,7 +13089,9 @@
       <c r="G17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="I17" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update du.xlsx (17 Nov)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\SECRET-BIOS\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DAB711-2FD4-4DB2-861C-73F2DABC2F66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F788357-838C-4884-8683-0644340DDE1B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="126">
   <si>
     <t>Question</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>Prepare for final submission and presentation slides</t>
+  </si>
+  <si>
+    <t>Final Submission</t>
   </si>
 </sst>
 </file>
@@ -12659,7 +12662,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12734,7 +12737,9 @@
       <c r="H3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -12759,7 +12764,9 @@
       <c r="H4" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
@@ -12784,7 +12791,9 @@
       <c r="H5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -12811,7 +12820,9 @@
       <c r="H6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
@@ -12836,7 +12847,9 @@
       <c r="H7" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
@@ -12861,7 +12874,9 @@
       <c r="H8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -12888,7 +12903,9 @@
       <c r="H9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
@@ -12913,7 +12930,9 @@
       <c r="H10" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
@@ -12938,7 +12957,9 @@
       <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
@@ -12965,7 +12986,9 @@
       <c r="H12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
@@ -12990,7 +13013,9 @@
       <c r="H13" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
@@ -13015,7 +13040,9 @@
       <c r="H14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -13042,7 +13069,9 @@
       <c r="H15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="7" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
@@ -13067,7 +13096,9 @@
       <c r="H16" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
@@ -13092,7 +13123,9 @@
       <c r="H17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>